<commit_message>
Public Holiday Export to Excel, Bulk Upload and Upload Template
</commit_message>
<xml_diff>
--- a/Client_CSILMS/src/templates/LeaveEntitlement.xlsx
+++ b/Client_CSILMS/src/templates/LeaveEntitlement.xlsx
@@ -172,9 +172,6 @@
     <t>You may contact the Development Team for further assistance of using this template.</t>
   </si>
   <si>
-    <t>Failing to follow any of the these below rules may result to unsuccessful upload of Entitlement data.</t>
-  </si>
-  <si>
     <t>This is the template for uploading the Leave Entitlements. Please be reminded with the following rules of filling in the values on each Column Field.</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>Initial Draft Template.</t>
+  </si>
+  <si>
+    <t>Failing to follow any of these below rules may result to unsuccessful upload of Entitlement data.</t>
   </si>
 </sst>
 </file>
@@ -969,12 +969,6 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
@@ -996,6 +990,12 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1322,7 +1322,7 @@
   <dimension ref="A1:I38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1348,99 +1348,99 @@
       <c r="A2" s="16"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B3" s="17" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="25" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="26"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="27"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="B3" s="19" t="s">
+      <c r="B4" s="20">
+        <v>43515</v>
+      </c>
+      <c r="C4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="C3" s="19" t="s">
-        <v>45</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="28"/>
-      <c r="F3" s="28"/>
-      <c r="G3" s="28"/>
-      <c r="H3" s="29"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="21" t="s">
-        <v>43</v>
-      </c>
-      <c r="B4" s="22">
-        <v>43515</v>
-      </c>
-      <c r="C4" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="24" t="s">
-        <v>47</v>
-      </c>
-      <c r="E4" s="25"/>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="26"/>
+      <c r="E4" s="23"/>
+      <c r="F4" s="23"/>
+      <c r="G4" s="23"/>
+      <c r="H4" s="24"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="21"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="25"/>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="26"/>
+      <c r="A5" s="19"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="18"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="23"/>
+      <c r="F5" s="23"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="24"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="20"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="25"/>
-      <c r="H6" s="26"/>
+      <c r="A6" s="18"/>
+      <c r="B6" s="18"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="23"/>
+      <c r="F6" s="23"/>
+      <c r="G6" s="23"/>
+      <c r="H6" s="24"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="23"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
+      <c r="A7" s="21"/>
+      <c r="B7" s="21"/>
+      <c r="C7" s="21"/>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21"/>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="23"/>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23"/>
-      <c r="F8" s="23"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="23"/>
+      <c r="A8" s="21"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21"/>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1481,122 +1481,122 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="18" t="s">
+      <c r="C21" s="29" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="18"/>
-      <c r="E21" s="18"/>
+      <c r="D21" s="29"/>
+      <c r="E21" s="29"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B22" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="17" t="s">
+      <c r="C22" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="D22" s="17"/>
-      <c r="E22" s="17"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B23" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="D23" s="17"/>
-      <c r="E23" s="17"/>
+      <c r="D23" s="28"/>
+      <c r="E23" s="28"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B24" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="17" t="s">
+      <c r="C24" s="28" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="17"/>
-      <c r="E24" s="17"/>
+      <c r="D24" s="28"/>
+      <c r="E24" s="28"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B25" s="15" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="28" t="s">
         <v>12</v>
       </c>
-      <c r="D25" s="17"/>
-      <c r="E25" s="17"/>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B26" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="17" t="s">
+      <c r="C26" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="17"/>
-      <c r="E26" s="17"/>
+      <c r="D26" s="28"/>
+      <c r="E26" s="28"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="28" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="17"/>
-      <c r="E27" s="17"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="28"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C28" s="17" t="s">
+      <c r="C28" s="28" t="s">
         <v>15</v>
       </c>
-      <c r="D28" s="17"/>
-      <c r="E28" s="17"/>
+      <c r="D28" s="28"/>
+      <c r="E28" s="28"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C29" s="17" t="s">
+      <c r="C29" s="28" t="s">
         <v>16</v>
       </c>
-      <c r="D29" s="17"/>
-      <c r="E29" s="17"/>
+      <c r="D29" s="28"/>
+      <c r="E29" s="28"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="17" t="s">
+      <c r="C30" s="28" t="s">
         <v>17</v>
       </c>
-      <c r="D30" s="17"/>
-      <c r="E30" s="17"/>
+      <c r="D30" s="28"/>
+      <c r="E30" s="28"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="17" t="s">
+      <c r="C31" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="17"/>
-      <c r="E31" s="17"/>
+      <c r="D31" s="28"/>
+      <c r="E31" s="28"/>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Translate Items, Upload Entitlement and Holidays, etc
</commit_message>
<xml_diff>
--- a/Client_CSILMS/src/templates/LeaveEntitlement.xlsx
+++ b/Client_CSILMS/src/templates/LeaveEntitlement.xlsx
@@ -142,6 +142,209 @@
     </r>
   </si>
   <si>
+    <t>if the Employee(s) doesn't have credits for any of those Leave Columns.</t>
+  </si>
+  <si>
+    <t>This is the template for uploading the Leave Entitlements. Please be reminded with the following rules of filling in the values on each Column Field.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.) This template contains eight (8) required column fields. Column Names or Headers shouldn't be missed or misspelled. </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Following below are the Column Names/Headers. Please verify that all of these are present in the </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Entitlement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> sheet with exact word, NO spaces in between.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Leave Type</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> values must be listed in below list of Leave Types:</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">5.) Leave Days for </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Carried Forward</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Entitlement</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Available Leave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Taken Leave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Balance Leave</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> must all have a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Number</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> values. Please fill in zero (0)</t>
+    </r>
+  </si>
+  <si>
+    <t>Version</t>
+  </si>
+  <si>
+    <t>1.0</t>
+  </si>
+  <si>
+    <t>Junnel Teves</t>
+  </si>
+  <si>
+    <t>Created By</t>
+  </si>
+  <si>
+    <t>Date Created</t>
+  </si>
+  <si>
+    <t>Initial Draft Template.</t>
+  </si>
+  <si>
+    <t>Failing to follow any of these below rules may result to unsuccessful upload of Entitlement data.</t>
+  </si>
+  <si>
+    <t>You may contact the Development Team for further assistance in using this template.</t>
+  </si>
+  <si>
+    <t>6.) As best practice, always download and use the most updated Upload Template available in the "Upload Leave Entitlements" page.</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">3.) </t>
     </r>
@@ -162,211 +365,8 @@
         <rFont val="Arial"/>
         <family val="2"/>
       </rPr>
-      <t xml:space="preserve"> values must be a valid Year (should be current or the approaching Year).</t>
-    </r>
-  </si>
-  <si>
-    <t>if the Employee(s) doesn't have credits for any of those Leave Columns.</t>
-  </si>
-  <si>
-    <t>This is the template for uploading the Leave Entitlements. Please be reminded with the following rules of filling in the values on each Column Field.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1.) This template contains eight (8) required column fields. Column Names or Headers shouldn't be missed or misspelled. </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Following below are the Column Names/Headers. Please verify that all of these are present in the </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Entitlement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> sheet with exact word, NO spaces in between.</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">4.) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Leave Type</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> values must be listed in below list of Leave Types:</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">5.) Leave Days for </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Carried Forward</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Entitlement</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Available Leave</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Taken Leave</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Balance Leave</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> must all have a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t>Number</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> values. Please fill in zero (0)</t>
-    </r>
-  </si>
-  <si>
-    <t>Version</t>
-  </si>
-  <si>
-    <t>1.0</t>
-  </si>
-  <si>
-    <t>Junnel Teves</t>
-  </si>
-  <si>
-    <t>Created By</t>
-  </si>
-  <si>
-    <t>Date Created</t>
-  </si>
-  <si>
-    <t>Initial Draft Template.</t>
-  </si>
-  <si>
-    <t>Failing to follow any of these below rules may result to unsuccessful upload of Entitlement data.</t>
-  </si>
-  <si>
-    <t>You may contact the Development Team for further assistance in using this template.</t>
-  </si>
-  <si>
-    <t>6.) As best practice, always download and use the most updated Upload Template available in the "Upload Leave Entitlements" page.</t>
+      <t xml:space="preserve"> values must be a 4-digit number and a valid Year (should be current or the approaching Year).</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1325,7 +1325,7 @@
   <dimension ref="A1:I37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G27" sqref="G27"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1352,13 +1352,13 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" s="17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D3" s="25" t="s">
         <v>31</v>
@@ -1370,16 +1370,16 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B4" s="20">
         <v>43515</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D4" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E4" s="23"/>
       <c r="F4" s="23"/>
@@ -1428,22 +1428,22 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -1479,12 +1479,12 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1599,22 +1599,22 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B34" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B37" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>